<commit_message>
movendo partes em comum para o modulo de commons
</commit_message>
<xml_diff>
--- a/products_teste_webdev_.xlsx
+++ b/products_teste_webdev_.xlsx
@@ -100,8 +100,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -175,12 +176,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -264,36 +273,38 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="27.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="27.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="1" t="n">
         <v>123123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -301,7 +312,7 @@
       <c r="A4" s="0" t="n">
         <v>1001</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -318,7 +329,7 @@
       <c r="A5" s="0" t="n">
         <v>1002</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -335,7 +346,7 @@
       <c r="A6" s="0" t="n">
         <v>1003</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -352,7 +363,7 @@
       <c r="A7" s="0" t="n">
         <v>1008</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -369,7 +380,7 @@
       <c r="A8" s="0" t="n">
         <v>1009</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -386,7 +397,7 @@
       <c r="A9" s="0" t="n">
         <v>1010</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="0" t="n">

</xml_diff>